<commit_message>
functions to estimate calculated contam concentrations
</commit_message>
<xml_diff>
--- a/data/raw/missing_other values.xlsx
+++ b/data/raw/missing_other values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\MarcusBeck\SQO_web\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76EFF18-F2E9-4C69-98EE-8FFE206835DE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737F3AF3-6E98-4030-AD72-2F8E353C6E7F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26955" yWindow="-720" windowWidth="19530" windowHeight="9360" xr2:uid="{B4F32A66-8632-4E55-A140-4F8E33CB5184}"/>
+    <workbookView xWindow="24735" yWindow="-735" windowWidth="22935" windowHeight="11790" xr2:uid="{B4F32A66-8632-4E55-A140-4F8E33CB5184}"/>
   </bookViews>
   <sheets>
     <sheet name="User inputs" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="191">
   <si>
     <t>PCB Congener</t>
   </si>
@@ -595,6 +595,18 @@
   </si>
   <si>
     <t>AssimEff 1, 2, and 3=alpha, beta, and chi</t>
+  </si>
+  <si>
+    <t>betap=lipcf</t>
+  </si>
+  <si>
+    <t>NLOC proportionality constant</t>
+  </si>
+  <si>
+    <t>beta=lipcfp</t>
+  </si>
+  <si>
+    <t>NLOM proportionality constant (MAF) (0.035)</t>
   </si>
 </sst>
 </file>
@@ -966,10 +978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8501A7EC-F8D5-4085-A68E-732C6487D591}">
-  <dimension ref="A1:D109"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D8" sqref="D8:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,12 +991,12 @@
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>132</v>
       </c>
@@ -995,7 +1007,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>134</v>
       </c>
@@ -1006,7 +1018,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -1017,7 +1029,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -1028,7 +1040,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -1039,7 +1051,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>142</v>
       </c>
@@ -1047,23 +1059,35 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>144</v>
       </c>
       <c r="B8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>187</v>
+      </c>
+      <c r="E8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>146</v>
       </c>
       <c r="B9" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>189</v>
+      </c>
+      <c r="E9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>148</v>
       </c>
@@ -1071,12 +1095,12 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>150</v>
       </c>
@@ -1084,7 +1108,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>151</v>
       </c>
@@ -1092,7 +1116,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>152</v>
       </c>

</xml_diff>